<commit_message>
subida url de videos
</commit_message>
<xml_diff>
--- a/Documentos/Agenda.xlsx
+++ b/Documentos/Agenda.xlsx
@@ -169,9 +169,6 @@
     <t>https://github.com/jmacboy/electiva-programacion-2016-2-nur</t>
   </si>
   <si>
-    <t>Por subir</t>
-  </si>
-  <si>
     <t>Por Definir</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>https://www.dropbox.com/sh/5at7dnsojdtvtv4/AADjyz26bhZeTcs5rqgiOQega?dl=0</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/sh/md6wge93fccp3tj/AAALRkINpNqVq6Od8OtwaV1Wa?dl=0</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="35"/>
     </row>
@@ -1306,7 +1306,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="42" t="s">
         <v>28</v>
@@ -1315,7 +1315,7 @@
         <v>17</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.35">
@@ -1342,7 +1342,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="42" t="s">
         <v>33</v>
@@ -1351,7 +1351,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.8" x14ac:dyDescent="0.35">
@@ -1418,7 +1418,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>42</v>
@@ -1435,7 +1435,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>43</v>
@@ -1452,7 +1452,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="42" t="s">
         <v>44</v>
@@ -1469,7 +1469,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>45</v>
@@ -1734,7 +1734,7 @@
   <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1774,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -1793,7 +1793,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.35">

</xml_diff>